<commit_message>
replaced Admin Center w/ Azure Portal throughout; revised partner csv
</commit_message>
<xml_diff>
--- a/microsoft-365/managed-desktop/get-started/downloads/downloads/device-registration-sample-partner.xlsx
+++ b/microsoft-365/managed-desktop/get-started/downloads/downloads/device-registration-sample-partner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaimeo\microsoft-365-docs-pr\microsoft-365\managed-desktop\get-started\downloads\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C8114CC-A97B-4BD8-9FD0-F9906483D973}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E57126-89FC-45EC-91B3-340AE7B6FC0C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-1380" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <t>SpiralOrbit,ContosoABC,000000000000,</t>
   </si>
   <si>
-    <t>Manufacturer,Model,Serial Number,</t>
+    <t>Manufacturer,Model,Serial Number,Hardware Hash</t>
   </si>
 </sst>
 </file>

</xml_diff>